<commit_message>
Change: Main to scripts
</commit_message>
<xml_diff>
--- a/data/custom_models.xlsx
+++ b/data/custom_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BlockGame\blockgame_texturepack\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70ABD24B-5F23-48A6-99EC-2BD7B0136E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121DB6BB-F762-48D2-AA9A-49FDE4B5786E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>custom_model_data</t>
   </si>
@@ -43,13 +43,19 @@
   </si>
   <si>
     <t>item/custom/backpack</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>..\texturepack\assets\minecraft\models\item\custom\backpack.bbmodel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +71,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -74,7 +88,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -91,15 +105,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -389,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,9 +439,10 @@
     <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -415,8 +455,11 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -429,8 +472,11 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -442,13 +488,20 @@
       </c>
       <c r="D3" t="s">
         <v>5</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{DB64AB03-99F6-4F37-9494-BA7334380C12}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{3B91F46C-D058-461B-B8C5-7ACDC57188E6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Feat: Working flat model
</commit_message>
<xml_diff>
--- a/data/custom_models.xlsx
+++ b/data/custom_models.xlsx
@@ -8,47 +8,91 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BlockGame\blockgame_texturepack\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121DB6BB-F762-48D2-AA9A-49FDE4B5786E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D34D1A7-1F66-4A8E-BF8C-976850FCCB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>custom_model_data</t>
   </si>
   <si>
-    <t>model</t>
-  </si>
-  <si>
     <t>item/iron_ingot</t>
   </si>
   <si>
-    <t>parent_item</t>
-  </si>
-  <si>
-    <t>model_location</t>
-  </si>
-  <si>
-    <t>item/custom/backpack</t>
-  </si>
-  <si>
-    <t>link</t>
-  </si>
-  <si>
     <t>..\texturepack\assets\minecraft\models\item\custom\backpack.bbmodel</t>
+  </si>
+  <si>
+    <t>internal_name</t>
+  </si>
+  <si>
+    <t>backpack</t>
+  </si>
+  <si>
+    <t>link_to_bbmodel</t>
+  </si>
+  <si>
+    <t>link_to_texture</t>
+  </si>
+  <si>
+    <t>..\texturepack\assets\blockgame\textures\backpack.png</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>item/bone</t>
+  </si>
+  <si>
+    <t>Animated Bone</t>
+  </si>
+  <si>
+    <t>original_item</t>
+  </si>
+  <si>
+    <t>item/backpack/backpack</t>
+  </si>
+  <si>
+    <t>item/bone_animated/bone_animated</t>
+  </si>
+  <si>
+    <t>..\texturepack\assets\minecraft\models\item\bone_animated\bone_animated.png</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>handheld</t>
+  </si>
+  <si>
+    <t>iron_ingot</t>
   </si>
 </sst>
 </file>
@@ -88,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -125,17 +169,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -428,80 +499,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="68.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="56.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2">
+        <v>123456789</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
+      <c r="F2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($B2,LEN($B2)-FIND("/",$B2)), "{CustomModelData:",$C2,"}")</f>
+        <v>/give @s minecraft:iron_ingot{CustomModelData:123456789}</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>123456789</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>123456780</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>547746584</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($B3,LEN($B3)-FIND("/",$B3)), "{CustomModelData:",$C3,"}")</f>
+        <v>/give @s minecraft:bone{CustomModelData:547746584}</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{DB64AB03-99F6-4F37-9494-BA7334380C12}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{3B91F46C-D058-461B-B8C5-7ACDC57188E6}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{DB64AB03-99F6-4F37-9494-BA7334380C12}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{17EC1C9E-1216-4005-8646-88EA1BFD06B7}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{20121373-70BD-4B5C-A4D1-F9BF1BD2C1F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: Redundant key in bone_animated.json
</commit_message>
<xml_diff>
--- a/data/custom_models.xlsx
+++ b/data/custom_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BlockGame\blockgame_texturepack\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A1FD99-0DC5-45B0-B2E4-F62D7AF3999D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81998572-BF5B-4A0B-922C-D2DF51E93491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Feat: Shield and Potion test
</commit_message>
<xml_diff>
--- a/data/custom_models.xlsx
+++ b/data/custom_models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BlockGame\blockgame_texturepack\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81998572-BF5B-4A0B-922C-D2DF51E93491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC022EC-9F76-4EC7-AFDE-0F258B5DFAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>custom_model_data</t>
   </si>
@@ -68,6 +68,9 @@
     <t>original_item</t>
   </si>
   <si>
+    <t>textures</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
@@ -77,6 +80,12 @@
     <t>blockgame:backpack/backpack</t>
   </si>
   <si>
+    <t>item/generated</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
     <t>..\texturepack\assets\blockgame\backpack\backpack.bbmodel</t>
   </si>
   <si>
@@ -87,6 +96,27 @@
   </si>
   <si>
     <t>../texturepack/assets/blockgame/models/bone_animated/bone_animated.json</t>
+  </si>
+  <si>
+    <t>item/shield</t>
+  </si>
+  <si>
+    <t>Copper Shield</t>
+  </si>
+  <si>
+    <t>blockgame:shield/shield_copper</t>
+  </si>
+  <si>
+    <t>item/potion</t>
+  </si>
+  <si>
+    <t>blockgame:potion/potion_custom</t>
+  </si>
+  <si>
+    <t>Custom Potion</t>
+  </si>
+  <si>
+    <t>{'layer0':'item/potion_overlay', 'layer1':'item/potion'}</t>
   </si>
 </sst>
 </file>
@@ -207,17 +237,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -504,103 +524,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="56.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="8" t="str">
+        <f>_xlfn.CONCAT("{'layer0':'",A2,"'}")</f>
+        <v>{'layer0':'item/iron_ingot'}</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="str">
-        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A2,LEN($A2)-FIND("/",$A2)), "{CustomModelData:",$B2,"}")</f>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A2,LEN($A2)-FIND("/",$A2)), "{CustomModelData:",$D2,"}")</f>
         <v>/give @s minecraft:iron_ingot{CustomModelData:1}</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <f>_xlfn.CONCAT("{'layer0':'",A3,"'}")</f>
+        <v>{'layer0':'item/bone'}</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A3,LEN($A3)-FIND("/",$A3)), "{CustomModelData:",$D3,"}")</f>
+        <v>/give @s minecraft:bone{CustomModelData:2}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="str">
-        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A3,LEN($A3)-FIND("/",$A3)), "{CustomModelData:",$B3,"}")</f>
-        <v>/give @s minecraft:bone{CustomModelData:2}</v>
+      <c r="C4" s="8" t="str">
+        <f>_xlfn.CONCAT("{'layer0':'",A4,"'}")</f>
+        <v>{'layer0':'item/shield'}</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A4,LEN($A4)-FIND("/",$A4)), "{CustomModelData:",$D4,"}")</f>
+        <v>/give @s minecraft:shield{CustomModelData:3}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A5,LEN($A5)-FIND("/",$A5)), "{CustomModelData:",$D5,"}")</f>
+        <v>/give @s minecraft:potion{CustomModelData:4}</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="..\texturepack\assets\minecraft\models\item\custom\backpack.bbmodel" xr:uid="{DB64AB03-99F6-4F37-9494-BA7334380C12}"/>
-    <hyperlink ref="F2" r:id="rId2" display="..\texturepack\assets\blockgame\textures\backpack.png" xr:uid="{17EC1C9E-1216-4005-8646-88EA1BFD06B7}"/>
-    <hyperlink ref="F3" r:id="rId3" display="..\texturepack\assets\minecraft\models\item\bone_animated\bone_animated.png" xr:uid="{20121373-70BD-4B5C-A4D1-F9BF1BD2C1F2}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{231B3D2F-D2D3-47EA-A4B9-C42D1BE049EA}"/>
+    <hyperlink ref="G2" r:id="rId1" display="..\texturepack\assets\minecraft\models\item\custom\backpack.bbmodel" xr:uid="{DB64AB03-99F6-4F37-9494-BA7334380C12}"/>
+    <hyperlink ref="H2" r:id="rId2" display="..\texturepack\assets\blockgame\textures\backpack.png" xr:uid="{17EC1C9E-1216-4005-8646-88EA1BFD06B7}"/>
+    <hyperlink ref="H3" r:id="rId3" display="..\texturepack\assets\minecraft\models\item\bone_animated\bone_animated.png" xr:uid="{20121373-70BD-4B5C-A4D1-F9BF1BD2C1F2}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{231B3D2F-D2D3-47EA-A4B9-C42D1BE049EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>

</xml_diff>

<commit_message>
Feat: Potion with custom model
</commit_message>
<xml_diff>
--- a/data/custom_models.xlsx
+++ b/data/custom_models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BlockGame\blockgame_texturepack\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC022EC-9F76-4EC7-AFDE-0F258B5DFAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6843D20-82DD-4DB0-A921-C99961E347C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16080" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,44 +36,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
-  <si>
-    <t>custom_model_data</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>item/iron_ingot</t>
   </si>
   <si>
-    <t>internal_name</t>
-  </si>
-  <si>
-    <t>backpack</t>
-  </si>
-  <si>
-    <t>link_to_bbmodel</t>
-  </si>
-  <si>
-    <t>link_to_texture</t>
-  </si>
-  <si>
-    <t>command</t>
-  </si>
-  <si>
     <t>item/bone</t>
   </si>
   <si>
     <t>Animated Bone</t>
   </si>
   <si>
-    <t>original_item</t>
-  </si>
-  <si>
-    <t>textures</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>blockgame:bone_animated/bone_animated</t>
   </si>
   <si>
@@ -83,21 +56,6 @@
     <t>item/generated</t>
   </si>
   <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>..\texturepack\assets\blockgame\backpack\backpack.bbmodel</t>
-  </si>
-  <si>
-    <t>..\texturepack\assets\blockgame\bone_animated\bone_animated.png</t>
-  </si>
-  <si>
-    <t>..\texturepack\assets\blockgame\backpack\backpack.png</t>
-  </si>
-  <si>
-    <t>../texturepack/assets/blockgame/models/bone_animated/bone_animated.json</t>
-  </si>
-  <si>
     <t>item/shield</t>
   </si>
   <si>
@@ -117,6 +75,51 @@
   </si>
   <si>
     <t>{'layer0':'item/potion_overlay', 'layer1':'item/potion'}</t>
+  </si>
+  <si>
+    <t>Verbose Name</t>
+  </si>
+  <si>
+    <t>Backpack</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Give Command</t>
+  </si>
+  <si>
+    <t>Minecraft Item</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Textures</t>
+  </si>
+  <si>
+    <t>Custom Model Data</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Link to BBMODEL</t>
+  </si>
+  <si>
+    <t>Link to JSON</t>
+  </si>
+  <si>
+    <t>Link to texture folder</t>
+  </si>
+  <si>
+    <t>item/ice</t>
   </si>
 </sst>
 </file>
@@ -156,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -174,29 +177,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -205,9 +186,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -222,16 +201,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -524,176 +499,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="9" max="9" width="65.140625" customWidth="1"/>
+    <col min="10" max="10" width="74.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="56.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="1" t="str">
+        <f>_xlfn.CONCAT("{'layer0':'",C2,"'}")</f>
+        <v>{'layer0':'item/iron_ingot'}</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="4" t="str">
+        <f>IF(B2="model",HYPERLINK(_xlfn.CONCAT("../texturepack/assets/",SUBSTITUTE(G2,":","/models/"),".bbmodel")),"")</f>
+        <v>../texturepack/assets/blockgame/models/backpack/backpack.bbmodel</v>
+      </c>
+      <c r="I2" s="4" t="str">
+        <f>HYPERLINK(_xlfn.CONCAT("../texturepack/assets/",SUBSTITUTE($G2,":","/models/"),".json"))</f>
+        <v>../texturepack/assets/blockgame/models/backpack/backpack.json</v>
+      </c>
+      <c r="J2" s="4" t="str">
+        <f>HYPERLINK(_xlfn.CONCAT("../texturepack/assets/",SUBSTITUTE($G2,":","/textures/"),".png"))</f>
+        <v>../texturepack/assets/blockgame/textures/backpack/backpack.png</v>
+      </c>
+      <c r="K2" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($C2,LEN($C2)-FIND("/",$C2)), "{CustomModelData:",$F2,"}")</f>
+        <v>/give @s minecraft:iron_ingot{CustomModelData:1}</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="str">
+        <f>_xlfn.CONCAT("{'layer0':'",C3,"'}")</f>
+        <v>{'layer0':'item/bone'}</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4" t="str">
+        <f>IF(B3="model",HYPERLINK(_xlfn.CONCAT("../texturepack/assets/",SUBSTITUTE(G3,":","/models/"),".bbmodel")),"")</f>
+        <v/>
+      </c>
+      <c r="I3" s="4" t="str">
+        <f t="shared" ref="I3:I4" si="0">HYPERLINK(_xlfn.CONCAT("../texturepack/assets/",SUBSTITUTE($G3,":","/models/"),".json"))</f>
+        <v>../texturepack/assets/blockgame/models/bone_animated/bone_animated.json</v>
+      </c>
+      <c r="J3" s="4" t="str">
+        <f>HYPERLINK(_xlfn.CONCAT("../texturepack/assets/",SUBSTITUTE($G3,":","/textures/"),".png"))</f>
+        <v>../texturepack/assets/blockgame/textures/bone_animated/bone_animated.png</v>
+      </c>
+      <c r="K3" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($C3,LEN($C3)-FIND("/",$C3)), "{CustomModelData:",$F3,"}")</f>
+        <v>/give @s minecraft:bone{CustomModelData:2}</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f>_xlfn.CONCAT("{'layer0':'",C4,"'}")</f>
+        <v>{'layer0':'item/shield'}</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="4" t="str">
+        <f t="shared" ref="H4:H5" si="1">IF(B4="model",HYPERLINK(_xlfn.CONCAT("../texturepack/assets/",SUBSTITUTE(G4,":","/models/"),".bbmodel")),"")</f>
+        <v>../texturepack/assets/blockgame/models/shield/shield_copper.bbmodel</v>
+      </c>
+      <c r="I4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>../texturepack/assets/blockgame/models/shield/shield_copper.json</v>
+      </c>
+      <c r="J4" s="4" t="str">
+        <f t="shared" ref="J4:J5" si="2">HYPERLINK(_xlfn.CONCAT("../texturepack/assets/",SUBSTITUTE($G4,":","/textures/"),".png"))</f>
+        <v>../texturepack/assets/blockgame/textures/shield/shield_copper.png</v>
+      </c>
+      <c r="K4" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($C4,LEN($C4)-FIND("/",$C4)), "{CustomModelData:",$F4,"}")</f>
+        <v>/give @s minecraft:shield{CustomModelData:3}</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
+      <c r="H5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>../texturepack/assets/blockgame/models/potion/potion_custom.bbmodel</v>
+      </c>
+      <c r="I5" s="4" t="str">
+        <f>HYPERLINK(_xlfn.CONCAT("../texturepack/assets/",SUBSTITUTE($G5,":","/models/"),".json"))</f>
+        <v>../texturepack/assets/blockgame/models/potion/potion_custom.json</v>
+      </c>
+      <c r="J5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>../texturepack/assets/blockgame/textures/potion/potion_custom.png</v>
+      </c>
+      <c r="K5" t="str">
+        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($C5,LEN($C5)-FIND("/",$C5)), "{CustomModelData:",$F5,"}")</f>
+        <v>/give @s minecraft:potion{CustomModelData:4}</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="8" t="str">
-        <f>_xlfn.CONCAT("{'layer0':'",A2,"'}")</f>
-        <v>{'layer0':'item/iron_ingot'}</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="str">
-        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A2,LEN($A2)-FIND("/",$A2)), "{CustomModelData:",$D2,"}")</f>
-        <v>/give @s minecraft:iron_ingot{CustomModelData:1}</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="8" t="str">
-        <f>_xlfn.CONCAT("{'layer0':'",A3,"'}")</f>
-        <v>{'layer0':'item/bone'}</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="str">
-        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A3,LEN($A3)-FIND("/",$A3)), "{CustomModelData:",$D3,"}")</f>
-        <v>/give @s minecraft:bone{CustomModelData:2}</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="8" t="str">
-        <f>_xlfn.CONCAT("{'layer0':'",A4,"'}")</f>
-        <v>{'layer0':'item/shield'}</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" t="str">
-        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A4,LEN($A4)-FIND("/",$A4)), "{CustomModelData:",$D4,"}")</f>
-        <v>/give @s minecraft:shield{CustomModelData:3}</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="str">
-        <f>_xlfn.CONCAT("/give @s minecraft:", RIGHT($A5,LEN($A5)-FIND("/",$A5)), "{CustomModelData:",$D5,"}")</f>
-        <v>/give @s minecraft:potion{CustomModelData:4}</v>
-      </c>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="..\texturepack\assets\minecraft\models\item\custom\backpack.bbmodel" xr:uid="{DB64AB03-99F6-4F37-9494-BA7334380C12}"/>
-    <hyperlink ref="H2" r:id="rId2" display="..\texturepack\assets\blockgame\textures\backpack.png" xr:uid="{17EC1C9E-1216-4005-8646-88EA1BFD06B7}"/>
-    <hyperlink ref="H3" r:id="rId3" display="..\texturepack\assets\minecraft\models\item\bone_animated\bone_animated.png" xr:uid="{20121373-70BD-4B5C-A4D1-F9BF1BD2C1F2}"/>
-    <hyperlink ref="G3" r:id="rId4" xr:uid="{231B3D2F-D2D3-47EA-A4B9-C42D1BE049EA}"/>
+    <hyperlink ref="J3:J5" r:id="rId1" display="..\texturepack\assets\blockgame\textures\backpack.png" xr:uid="{A7BEEF28-8751-4C4E-9F14-2B3F069C5D04}"/>
+    <hyperlink ref="J2" r:id="rId2" display="..\texturepack\assets\blockgame\textures\backpack.png" xr:uid="{32940E91-7E5C-4776-BA14-2F71B27AA659}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>